<commit_message>
Make power plant fuel shifting calcs account for subsidies and prevent unintended reverse shifting (#22)
</commit_message>
<xml_diff>
--- a/InputData/elec/EoPPFTSwFP/Elasticity of Power Plant Fuel Type Shifting wrt Fuel Price.xlsx
+++ b/InputData/elec/EoPPFTSwFP/Elasticity of Power Plant Fuel Type Shifting wrt Fuel Price.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code Repositories\eps-us\InputData\elec\EoPPFTSwFP\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="120" windowWidth="27795" windowHeight="11325"/>
   </bookViews>
@@ -10,12 +15,12 @@
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="EoPPFTSwFP" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="70">
   <si>
     <t>EoPPFTSwFP Elasticity of Power Plant Fuel Type Shifting wrt Fuel Price</t>
   </si>
@@ -185,11 +190,111 @@
   <si>
     <t>pricing pressure, not elasticity values that represent the final steady</t>
   </si>
+  <si>
+    <t>Note that shifts are one-directional, from the source electricity fuel</t>
+  </si>
+  <si>
+    <t>(specified in a row here) to the target electricity fuel (specified in</t>
+  </si>
+  <si>
+    <t>a column here).  If the source type becomes more expensive, the</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">shift occurs.  If the source type becomes cheaper, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>nothing happens</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <t>because we cannot assume that shifts may occur bi-directionally.</t>
+  </si>
+  <si>
+    <t>(We cannot assume that because a plant may shift from coal to</t>
+  </si>
+  <si>
+    <t>natural gas, it would be able to shift back to coal.)</t>
+  </si>
+  <si>
+    <t>shift in the appropriate cell here (where the type being</t>
+  </si>
+  <si>
+    <t>shifted back from is the row and the type being shifted</t>
+  </si>
+  <si>
+    <t>back to is the column).</t>
+  </si>
+  <si>
+    <t>Shifts are one-directional</t>
+  </si>
+  <si>
+    <t>Even if a target fuel becomes cheaper than in the BAU case,</t>
+  </si>
+  <si>
+    <t>source plant types cause shifting.</t>
+  </si>
+  <si>
+    <t>Shifts are based on price increases, not decreases</t>
+  </si>
+  <si>
+    <t>this will not drive fuel shifting if the source plant type's dispatch</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">cost remains the same.  Only </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>increases</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> in the dispatch cost of</t>
+    </r>
+  </si>
+  <si>
+    <t>How to use this variable</t>
+  </si>
+  <si>
+    <t>If you want to allow bi-directional shifting, specify the other-direction</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -207,7 +312,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -226,6 +331,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -239,7 +350,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -262,6 +373,8 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -271,6 +384,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -319,7 +435,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -354,7 +470,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -563,7 +679,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B46"/>
+  <dimension ref="A1:E67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -617,129 +733,227 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="B30" s="11"/>
+      <c r="C30" s="11"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>44</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>46</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>47</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>37</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="B49" s="11"/>
+      <c r="C49" s="11"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="B63" s="11"/>
+      <c r="C63" s="11"/>
+      <c r="D63" s="11"/>
+      <c r="E63" s="11"/>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Base power plant fuel type shifting on perc dispatch cost changes for source-target plant type pairs (#22)
</commit_message>
<xml_diff>
--- a/InputData/elec/EoPPFTSwFP/Elasticity of Power Plant Fuel Type Shifting wrt Fuel Price.xlsx
+++ b/InputData/elec/EoPPFTSwFP/Elasticity of Power Plant Fuel Type Shifting wrt Fuel Price.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="66">
   <si>
     <t>EoPPFTSwFP Elasticity of Power Plant Fuel Type Shifting wrt Fuel Price</t>
   </si>
@@ -131,18 +131,6 @@
   </si>
   <si>
     <t>The rows also represent the plant types whose fuel cost is changing.</t>
-  </si>
-  <si>
-    <t>Values in orange cells are obtained from formulas that ensure</t>
-  </si>
-  <si>
-    <t>shifted plant capacity is properly removed from the former type.</t>
-  </si>
-  <si>
-    <t>calculate the corresponding reduction in the source plant type.</t>
-  </si>
-  <si>
-    <t>number between 0 and 0.2.  The orance cells will automatically</t>
   </si>
   <si>
     <t>so pick modest elasticity values that reflect gradual behavior response to</t>
@@ -204,47 +192,6 @@
     <t>back to is the column).</t>
   </si>
   <si>
-    <t>Shifts are one-directional</t>
-  </si>
-  <si>
-    <t>Even if a target fuel becomes cheaper than in the BAU case,</t>
-  </si>
-  <si>
-    <t>source plant types cause shifting.</t>
-  </si>
-  <si>
-    <t>Shifts are based on price increases, not decreases</t>
-  </si>
-  <si>
-    <t>this will not drive fuel shifting if the source plant type's dispatch</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">cost remains the same.  Only </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>increases</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> in the dispatch cost of</t>
-    </r>
-  </si>
-  <si>
     <t>How to use this variable</t>
   </si>
   <si>
@@ -295,6 +242,18 @@
       </rPr>
       <t>positive</t>
     </r>
+  </si>
+  <si>
+    <t>number between 0 and 0.2.</t>
+  </si>
+  <si>
+    <t>Gray-colored cells (the same power plant type as source and target)</t>
+  </si>
+  <si>
+    <t>should always be zero.</t>
+  </si>
+  <si>
+    <t>Shifts are one-directional unless both directions are specified</t>
   </si>
 </sst>
 </file>
@@ -318,7 +277,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -328,12 +287,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -376,11 +329,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -685,11 +638,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E71"/>
+  <dimension ref="A1:C64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="57.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -728,42 +684,42 @@
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
@@ -802,11 +758,11 @@
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="B33" s="11"/>
-      <c r="C33" s="11"/>
+      <c r="A33" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B33" s="10"/>
+      <c r="C33" s="4"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
@@ -825,153 +781,119 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>38</v>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>33</v>
+        <v>61</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>39</v>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
         <v>30</v>
       </c>
     </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="B52" s="10"/>
+      <c r="C52" s="4"/>
+    </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="B53" s="11"/>
-      <c r="C53" s="11"/>
+      <c r="A53" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>49</v>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="B67" s="11"/>
-      <c r="C67" s="11"/>
-      <c r="D67" s="11"/>
-      <c r="E67" s="11"/>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1060,9 +982,8 @@
       <c r="A2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="9">
-        <f>-SUM(C2:Q2)</f>
-        <v>-0.1</v>
+      <c r="B2" s="11">
+        <v>0</v>
       </c>
       <c r="C2" s="3">
         <v>0.1</v>
@@ -1117,8 +1038,7 @@
       <c r="B3" s="8">
         <v>0</v>
       </c>
-      <c r="C3" s="9">
-        <f>-SUM(B3,D3:Q3)</f>
+      <c r="C3" s="11">
         <v>0</v>
       </c>
       <c r="D3" s="8">
@@ -1174,8 +1094,7 @@
       <c r="C4" s="8">
         <v>0</v>
       </c>
-      <c r="D4" s="9">
-        <f>SUM(B4:C4,E4:Q4)</f>
+      <c r="D4" s="11">
         <v>0</v>
       </c>
       <c r="E4" s="2">
@@ -1231,8 +1150,7 @@
       <c r="D5" s="2">
         <v>0</v>
       </c>
-      <c r="E5" s="9">
-        <f>-SUM(B5:D5,F5:Q5)</f>
+      <c r="E5" s="11">
         <v>0</v>
       </c>
       <c r="F5" s="2">
@@ -1288,8 +1206,7 @@
       <c r="E6" s="2">
         <v>0</v>
       </c>
-      <c r="F6" s="9">
-        <f>-SUM(B6:E6,G6:Q6)</f>
+      <c r="F6" s="11">
         <v>0</v>
       </c>
       <c r="G6" s="2">
@@ -1345,8 +1262,7 @@
       <c r="F7" s="2">
         <v>0</v>
       </c>
-      <c r="G7" s="9">
-        <f>-SUM(B7:F7,H7:Q7)</f>
+      <c r="G7" s="11">
         <v>0</v>
       </c>
       <c r="H7" s="2">
@@ -1402,8 +1318,7 @@
       <c r="G8" s="2">
         <v>0</v>
       </c>
-      <c r="H8" s="9">
-        <f>-SUM(B8:G8,I8:Q8)</f>
+      <c r="H8" s="11">
         <v>0</v>
       </c>
       <c r="I8" s="2">
@@ -1459,8 +1374,7 @@
       <c r="H9" s="2">
         <v>0</v>
       </c>
-      <c r="I9" s="9">
-        <f>-SUM(B9:H9,J9:Q9)</f>
+      <c r="I9" s="11">
         <v>0</v>
       </c>
       <c r="J9" s="2">
@@ -1516,8 +1430,7 @@
       <c r="I10" s="2">
         <v>0</v>
       </c>
-      <c r="J10" s="9">
-        <f>-SUM(B10:I10,K10:Q10)</f>
+      <c r="J10" s="11">
         <v>0</v>
       </c>
       <c r="K10" s="2">
@@ -1573,8 +1486,7 @@
       <c r="J11" s="2">
         <v>0</v>
       </c>
-      <c r="K11" s="9">
-        <f>-SUM(B11:J11,L11:Q11)</f>
+      <c r="K11" s="11">
         <v>0</v>
       </c>
       <c r="L11" s="8">
@@ -1630,8 +1542,7 @@
       <c r="K12" s="2">
         <v>0</v>
       </c>
-      <c r="L12" s="9">
-        <f>-SUM(B12:K12,M12:Q12)</f>
+      <c r="L12" s="11">
         <v>0</v>
       </c>
       <c r="M12" s="2">
@@ -1687,8 +1598,7 @@
       <c r="L13" s="8">
         <v>0</v>
       </c>
-      <c r="M13" s="9">
-        <f>-SUM(B13:L13,N13:Q13)</f>
+      <c r="M13" s="11">
         <v>0</v>
       </c>
       <c r="N13" s="2">
@@ -1744,8 +1654,7 @@
       <c r="M14" s="2">
         <v>0</v>
       </c>
-      <c r="N14" s="9">
-        <f>-SUM(B14:M14,O14:Q14)</f>
+      <c r="N14" s="11">
         <v>0</v>
       </c>
       <c r="O14" s="2">
@@ -1801,8 +1710,7 @@
       <c r="N15" s="2">
         <v>0</v>
       </c>
-      <c r="O15" s="9">
-        <f>-SUM(B15:N15,P15:Q15)</f>
+      <c r="O15" s="11">
         <v>0</v>
       </c>
       <c r="P15" s="3">
@@ -1858,8 +1766,7 @@
       <c r="O16" s="3">
         <v>0</v>
       </c>
-      <c r="P16" s="9">
-        <f>-SUM(B16:O16,Q16)</f>
+      <c r="P16" s="11">
         <v>0</v>
       </c>
       <c r="Q16" s="2">
@@ -1915,8 +1822,7 @@
       <c r="P17" s="2">
         <v>0</v>
       </c>
-      <c r="Q17" s="9">
-        <f>-SUM(B17:P17)</f>
+      <c r="Q17" s="11">
         <v>0</v>
       </c>
     </row>

</xml_diff>